<commit_message>
updated project assign sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94DC1C2-D329-4126-986B-A13B7B2A38BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B49B4A-890F-494B-BB95-2BBC34B4AE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="247">
   <si>
     <t>owner</t>
   </si>
@@ -760,6 +760,12 @@
   </si>
   <si>
     <t>Keye Li</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>finished</t>
   </si>
 </sst>
 </file>
@@ -15796,10 +15802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B243"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15807,323 +15813,404 @@
     <col min="1" max="1" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>243</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -16293,7 +16380,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -16343,12 +16430,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -16388,7 +16475,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -16443,7 +16530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -16488,7 +16575,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -16508,7 +16595,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -16518,12 +16605,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
@@ -16563,7 +16650,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -16638,7 +16725,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
@@ -16653,7 +16740,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
@@ -16693,7 +16780,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -16773,7 +16860,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
@@ -16873,7 +16960,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
@@ -17008,85 +17095,88 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B229" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C229" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>239</v>
       </c>

</xml_diff>

<commit_message>
updated project assignment file
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\Summer Research\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E779B5F0-FBDB-492A-A1DC-0984127EDF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4120A1-7C3B-4528-B25B-DCF960279C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="254">
   <si>
     <t>project name</t>
   </si>
@@ -784,6 +784,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>can't import</t>
   </si>
 </sst>
 </file>
@@ -11587,14 +11590,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N69" sqref="N69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -11811,7 +11814,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -11822,7 +11825,7 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -11899,7 +11902,7 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -11965,7 +11968,7 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -12225,113 +12228,239 @@
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="B61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="B62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
update ownership for projects'
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wx199\mock-usage\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4120A1-7C3B-4528-B25B-DCF960279C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212977F6-CA45-4A07-B0E5-19DC3D23C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="275">
   <si>
     <t>project name</t>
   </si>
@@ -787,6 +787,69 @@
   </si>
   <si>
     <t>can't import</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>commons-vfs</t>
+  </si>
+  <si>
+    <t>commons-weaver</t>
+  </si>
+  <si>
+    <t>ant-antlibs-compress</t>
+  </si>
+  <si>
+    <t>continuum</t>
+  </si>
+  <si>
+    <t>cordova</t>
+  </si>
+  <si>
+    <t>crunch</t>
+  </si>
+  <si>
+    <t>ctakes</t>
+  </si>
+  <si>
+    <t>curator</t>
+  </si>
+  <si>
+    <t>cxf</t>
+  </si>
+  <si>
+    <t>daffodil</t>
+  </si>
+  <si>
+    <t>datafu</t>
+  </si>
+  <si>
+    <t>deltaspike</t>
+  </si>
+  <si>
+    <t>derby</t>
+  </si>
+  <si>
+    <t>directmemory</t>
+  </si>
+  <si>
+    <t>drill</t>
+  </si>
+  <si>
+    <t>ecs</t>
+  </si>
+  <si>
+    <t>devicemap-browsermap</t>
+  </si>
+  <si>
+    <t>directory-server</t>
+  </si>
+  <si>
+    <t>directory-studio</t>
+  </si>
+  <si>
+    <t>directory-ldap-api</t>
   </si>
 </sst>
 </file>
@@ -11588,19 +11651,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C243"/>
+  <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N69" sqref="N69"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="35.90625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11611,7 +11674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -11622,7 +11685,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11633,7 +11696,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11644,7 +11707,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11655,7 +11718,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -11666,7 +11729,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11677,7 +11740,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11688,7 +11751,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11696,7 +11759,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11707,7 +11770,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -11718,7 +11781,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -11729,7 +11792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -11740,7 +11803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -11751,7 +11814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -11762,7 +11825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -11773,7 +11836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -11784,7 +11847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -11795,7 +11858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -11806,7 +11869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -11817,7 +11880,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -11828,7 +11891,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11839,7 +11902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -11850,7 +11913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -11861,7 +11924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -11872,7 +11935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -11883,7 +11946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -11894,7 +11957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -11905,7 +11968,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -11916,7 +11979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -11927,7 +11990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -11938,7 +12001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -11949,7 +12012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -11960,7 +12023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -11971,7 +12034,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -11982,7 +12045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -11993,7 +12056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -12004,7 +12067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -12012,219 +12075,219 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -12235,7 +12298,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -12246,7 +12309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -12257,7 +12320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -12268,7 +12331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -12279,7 +12342,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
@@ -12290,7 +12353,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
@@ -12301,7 +12364,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -12312,7 +12375,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -12323,7 +12386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -12334,7 +12397,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
@@ -12345,7 +12408,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -12356,7 +12419,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
@@ -12367,7 +12430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -12378,7 +12441,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -12389,7 +12452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -12400,7 +12463,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -12411,7 +12474,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -12422,7 +12485,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -12433,7 +12496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -12444,7 +12507,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
@@ -12455,582 +12518,762 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D83" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D84" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D86" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D87" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D88" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D89" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D90" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D91" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D92" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D93" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D94" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D95" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D97" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D98" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>199</v>
       </c>
@@ -13041,12 +13284,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>201</v>
       </c>
@@ -13057,7 +13300,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>202</v>
       </c>
@@ -13068,7 +13311,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>203</v>
       </c>
@@ -13079,7 +13322,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>204</v>
       </c>
@@ -13090,7 +13333,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>205</v>
       </c>
@@ -13101,7 +13344,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>206</v>
       </c>
@@ -13112,7 +13355,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>207</v>
       </c>
@@ -13123,7 +13366,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>208</v>
       </c>
@@ -13134,7 +13377,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>209</v>
       </c>
@@ -13145,7 +13388,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>210</v>
       </c>
@@ -13156,7 +13399,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>211</v>
       </c>
@@ -13167,7 +13410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>212</v>
       </c>
@@ -13178,7 +13421,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>213</v>
       </c>
@@ -13189,7 +13432,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>214</v>
       </c>
@@ -13200,7 +13443,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>215</v>
       </c>
@@ -13211,7 +13454,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>216</v>
       </c>
@@ -13222,7 +13465,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>217</v>
       </c>
@@ -13233,7 +13476,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>218</v>
       </c>
@@ -13244,7 +13487,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>219</v>
       </c>
@@ -13255,7 +13498,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>220</v>
       </c>
@@ -13266,7 +13509,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>221</v>
       </c>
@@ -13277,7 +13520,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>222</v>
       </c>
@@ -13288,7 +13531,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>223</v>
       </c>
@@ -13296,7 +13539,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>224</v>
       </c>
@@ -13307,7 +13550,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>225</v>
       </c>
@@ -13318,7 +13561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>226</v>
       </c>
@@ -13329,7 +13572,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>227</v>
       </c>
@@ -13340,7 +13583,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>228</v>
       </c>
@@ -13348,12 +13591,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>230</v>
       </c>
@@ -13364,7 +13607,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>231</v>
       </c>
@@ -13375,7 +13618,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>232</v>
       </c>
@@ -13386,7 +13629,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>233</v>
       </c>
@@ -13397,7 +13640,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>234</v>
       </c>
@@ -13408,7 +13651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>235</v>
       </c>
@@ -13419,7 +13662,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>236</v>
       </c>
@@ -13430,12 +13673,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>238</v>
       </c>
@@ -13443,7 +13686,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>239</v>
       </c>
@@ -13454,7 +13697,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>240</v>
       </c>
@@ -13465,22 +13708,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>244</v>
       </c>
@@ -13491,7 +13734,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>245</v>
       </c>
@@ -13502,12 +13745,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>247</v>
       </c>
@@ -13518,7 +13761,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>248</v>
       </c>

</xml_diff>

<commit_message>
updated data folder structure and script
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4120A1-7C3B-4528-B25B-DCF960279C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07229BBA-FDD7-4421-82B0-F6B33B1EE113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="255">
   <si>
     <t>project name</t>
   </si>
@@ -787,6 +787,9 @@
   </si>
   <si>
     <t>can't import</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -11591,7 +11594,7 @@
   <dimension ref="A1:C243"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N69" sqref="N69"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12232,7 +12235,7 @@
         <v>14</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -12243,7 +12246,7 @@
         <v>14</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -12254,7 +12257,7 @@
         <v>14</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -12265,7 +12268,7 @@
         <v>14</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -12276,7 +12279,7 @@
         <v>14</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -12287,7 +12290,7 @@
         <v>14</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -12298,7 +12301,7 @@
         <v>14</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -12309,7 +12312,7 @@
         <v>14</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -12320,7 +12323,7 @@
         <v>14</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -12331,7 +12334,7 @@
         <v>14</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -12342,7 +12345,7 @@
         <v>14</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -12353,7 +12356,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -12364,7 +12367,7 @@
         <v>14</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -12375,7 +12378,7 @@
         <v>14</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -12386,7 +12389,7 @@
         <v>14</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -12397,7 +12400,7 @@
         <v>14</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -12408,7 +12411,7 @@
         <v>14</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -12419,7 +12422,7 @@
         <v>14</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -12430,7 +12433,7 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -12441,7 +12444,7 @@
         <v>14</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -12452,7 +12455,7 @@
         <v>14</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>43</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Another update for project assignment sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wx199\mock-usage\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212977F6-CA45-4A07-B0E5-19DC3D23C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DF506E-9CC1-4350-8E21-58CA981C0CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11653,17 +11653,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.90625" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11674,7 +11674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -11685,7 +11685,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11696,7 +11696,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11718,7 +11718,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11740,7 +11740,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11770,7 +11770,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -11781,7 +11781,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -11814,7 +11814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -11858,7 +11858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -11880,7 +11880,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11902,7 +11902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -11913,7 +11913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -11935,7 +11935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -11957,7 +11957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -11990,7 +11990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -12012,7 +12012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -12023,7 +12023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -12034,7 +12034,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -12056,7 +12056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -12089,7 +12089,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -12100,7 +12100,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -12111,7 +12111,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -12122,7 +12122,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -12144,7 +12144,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -12166,7 +12166,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -12188,7 +12188,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -12199,7 +12199,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -12210,7 +12210,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -12232,7 +12232,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -12254,7 +12254,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -12265,7 +12265,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -12287,7 +12287,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -12295,10 +12295,10 @@
         <v>14</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -12306,10 +12306,10 @@
         <v>14</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -12317,10 +12317,10 @@
         <v>14</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -12328,10 +12328,10 @@
         <v>14</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -12339,10 +12339,10 @@
         <v>14</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
@@ -12350,10 +12350,10 @@
         <v>14</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
@@ -12361,10 +12361,10 @@
         <v>14</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -12372,10 +12372,10 @@
         <v>14</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -12383,10 +12383,10 @@
         <v>14</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -12394,10 +12394,10 @@
         <v>14</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
@@ -12405,10 +12405,10 @@
         <v>14</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -12416,10 +12416,10 @@
         <v>14</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
@@ -12427,10 +12427,10 @@
         <v>14</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -12438,10 +12438,10 @@
         <v>14</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -12449,10 +12449,10 @@
         <v>14</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -12460,10 +12460,10 @@
         <v>14</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -12471,10 +12471,10 @@
         <v>14</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -12482,10 +12482,10 @@
         <v>14</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -12493,10 +12493,10 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -12504,10 +12504,10 @@
         <v>14</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
@@ -12515,10 +12515,10 @@
         <v>14</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
@@ -12532,7 +12532,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -12546,7 +12546,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>86</v>
       </c>
@@ -12560,7 +12560,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>87</v>
       </c>
@@ -12574,7 +12574,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>88</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>89</v>
       </c>
@@ -12602,7 +12602,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>90</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>91</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>92</v>
       </c>
@@ -12644,7 +12644,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>93</v>
       </c>
@@ -12658,7 +12658,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>94</v>
       </c>
@@ -12672,7 +12672,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>95</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>96</v>
       </c>
@@ -12700,7 +12700,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>97</v>
       </c>
@@ -12714,7 +12714,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>98</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>99</v>
       </c>
@@ -12742,7 +12742,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>100</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>101</v>
       </c>
@@ -12770,7 +12770,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>102</v>
       </c>
@@ -12784,7 +12784,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>103</v>
       </c>
@@ -12798,482 +12798,482 @@
         <v>270</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>199</v>
       </c>
@@ -13284,12 +13284,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>201</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>202</v>
       </c>
@@ -13311,7 +13311,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>203</v>
       </c>
@@ -13322,7 +13322,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>204</v>
       </c>
@@ -13333,7 +13333,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>205</v>
       </c>
@@ -13344,7 +13344,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>206</v>
       </c>
@@ -13355,7 +13355,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>207</v>
       </c>
@@ -13366,7 +13366,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>208</v>
       </c>
@@ -13377,7 +13377,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>209</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>210</v>
       </c>
@@ -13399,7 +13399,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>211</v>
       </c>
@@ -13410,7 +13410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>212</v>
       </c>
@@ -13421,7 +13421,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>213</v>
       </c>
@@ -13432,7 +13432,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>214</v>
       </c>
@@ -13443,7 +13443,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>215</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>216</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>217</v>
       </c>
@@ -13476,7 +13476,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>218</v>
       </c>
@@ -13487,7 +13487,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>219</v>
       </c>
@@ -13498,7 +13498,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>220</v>
       </c>
@@ -13509,7 +13509,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>221</v>
       </c>
@@ -13520,7 +13520,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>222</v>
       </c>
@@ -13531,7 +13531,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>223</v>
       </c>
@@ -13539,7 +13539,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>224</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>225</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>226</v>
       </c>
@@ -13572,7 +13572,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>227</v>
       </c>
@@ -13583,7 +13583,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>228</v>
       </c>
@@ -13591,12 +13591,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>230</v>
       </c>
@@ -13607,7 +13607,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>231</v>
       </c>
@@ -13618,7 +13618,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>232</v>
       </c>
@@ -13629,7 +13629,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>233</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>234</v>
       </c>
@@ -13651,7 +13651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>235</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>236</v>
       </c>
@@ -13673,12 +13673,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>238</v>
       </c>
@@ -13686,7 +13686,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>239</v>
       </c>
@@ -13697,7 +13697,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>240</v>
       </c>
@@ -13708,22 +13708,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>244</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>245</v>
       </c>
@@ -13745,12 +13745,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>247</v>
       </c>
@@ -13761,7 +13761,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>248</v>
       </c>

</xml_diff>

<commit_message>
Updated project assignment sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wx199\mock-usage\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\Summer Research\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA0A2F-DF34-4DB3-9D77-241BD3D8D00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD24E24A-7671-4135-B4F9-B19C648FE817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="275">
   <si>
     <t>project name</t>
   </si>
@@ -778,9 +778,6 @@
   </si>
   <si>
     <t>No Git Repo</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>can't import</t>
@@ -11656,17 +11653,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.90625" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11677,7 +11674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -11688,7 +11685,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11699,7 +11696,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11710,7 +11707,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11721,7 +11718,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -11732,7 +11729,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11743,7 +11740,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11754,7 +11751,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11762,7 +11759,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11773,7 +11770,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -11784,7 +11781,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -11795,7 +11792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -11806,7 +11803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -11817,7 +11814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -11828,7 +11825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -11839,7 +11836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -11850,7 +11847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -11861,7 +11858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -11872,7 +11869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -11883,7 +11880,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -11891,10 +11888,10 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11905,7 +11902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -11916,7 +11913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -11927,7 +11924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -11938,7 +11935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -11949,7 +11946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -11960,7 +11957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -11968,10 +11965,10 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -11982,7 +11979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -11993,7 +11990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -12004,7 +12001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -12015,7 +12012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -12026,7 +12023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -12034,10 +12031,10 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -12048,7 +12045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -12059,7 +12056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -12070,7 +12067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -12078,10 +12075,10 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -12089,10 +12086,10 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -12100,10 +12097,10 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -12111,10 +12108,10 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -12122,10 +12119,10 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -12133,10 +12130,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -12144,10 +12141,10 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -12155,10 +12152,10 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -12166,10 +12163,10 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -12177,10 +12174,10 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -12188,10 +12185,10 @@
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -12199,10 +12196,10 @@
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -12210,10 +12207,10 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -12221,10 +12218,10 @@
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -12232,10 +12229,10 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -12243,10 +12240,10 @@
         <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -12254,10 +12251,10 @@
         <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -12265,10 +12262,10 @@
         <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -12276,10 +12273,10 @@
         <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -12287,10 +12284,10 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -12298,10 +12295,10 @@
         <v>14</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -12309,10 +12306,10 @@
         <v>14</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -12320,10 +12317,10 @@
         <v>14</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -12331,10 +12328,10 @@
         <v>14</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -12342,10 +12339,10 @@
         <v>14</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -12353,10 +12350,10 @@
         <v>14</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -12364,10 +12361,10 @@
         <v>14</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -12375,10 +12372,10 @@
         <v>14</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -12386,10 +12383,10 @@
         <v>14</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -12397,10 +12394,10 @@
         <v>14</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -12408,10 +12405,10 @@
         <v>14</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -12419,10 +12416,10 @@
         <v>14</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -12430,10 +12427,10 @@
         <v>14</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -12441,10 +12438,10 @@
         <v>14</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -12452,10 +12449,10 @@
         <v>14</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -12463,10 +12460,10 @@
         <v>14</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -12474,10 +12471,10 @@
         <v>14</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -12485,10 +12482,10 @@
         <v>14</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -12496,10 +12493,10 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -12507,10 +12504,10 @@
         <v>14</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -12518,10 +12515,10 @@
         <v>14</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -12529,13 +12526,13 @@
         <v>42</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D79" t="s">
         <v>253</v>
       </c>
-      <c r="D79" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -12543,13 +12540,13 @@
         <v>42</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D80" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -12557,13 +12554,13 @@
         <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D81" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -12571,13 +12568,13 @@
         <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D82" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -12585,13 +12582,13 @@
         <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D83" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -12599,13 +12596,13 @@
         <v>42</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D84" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -12613,13 +12610,13 @@
         <v>42</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D85" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -12627,13 +12624,13 @@
         <v>42</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -12641,13 +12638,13 @@
         <v>42</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D87" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -12655,13 +12652,13 @@
         <v>42</v>
       </c>
       <c r="C88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D88" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -12669,13 +12666,13 @@
         <v>42</v>
       </c>
       <c r="C89" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D89" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -12683,13 +12680,13 @@
         <v>42</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D90" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -12697,13 +12694,13 @@
         <v>42</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D91" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -12711,13 +12708,13 @@
         <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D92" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -12725,13 +12722,13 @@
         <v>42</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D93" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -12739,13 +12736,13 @@
         <v>42</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D94" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -12753,13 +12750,13 @@
         <v>42</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D95" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -12767,13 +12764,13 @@
         <v>42</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D96" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -12781,13 +12778,13 @@
         <v>42</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D97" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -12798,485 +12795,545 @@
         <v>250</v>
       </c>
       <c r="D98" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B181" t="s">
+        <v>248</v>
+      </c>
+      <c r="C181" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B182" t="s">
+        <v>248</v>
+      </c>
+      <c r="C182" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B183" t="s">
+        <v>248</v>
+      </c>
+      <c r="C183" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B185" t="s">
+        <v>248</v>
+      </c>
+      <c r="C185" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B186" t="s">
+        <v>248</v>
+      </c>
+      <c r="C186" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B187" t="s">
+        <v>248</v>
+      </c>
+      <c r="C187" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B188" t="s">
+        <v>248</v>
+      </c>
+      <c r="C188" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B190" t="s">
+        <v>248</v>
+      </c>
+      <c r="C190" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B192" t="s">
+        <v>248</v>
+      </c>
+      <c r="C192" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B193" t="s">
+        <v>248</v>
+      </c>
+      <c r="C193" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
@@ -13284,15 +13341,15 @@
         <v>248</v>
       </c>
       <c r="C194" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
@@ -13300,10 +13357,10 @@
         <v>248</v>
       </c>
       <c r="C196" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
@@ -13311,10 +13368,10 @@
         <v>248</v>
       </c>
       <c r="C197" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
@@ -13322,10 +13379,10 @@
         <v>248</v>
       </c>
       <c r="C198" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
@@ -13333,10 +13390,10 @@
         <v>248</v>
       </c>
       <c r="C199" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
@@ -13344,10 +13401,10 @@
         <v>248</v>
       </c>
       <c r="C200" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
@@ -13355,10 +13412,10 @@
         <v>248</v>
       </c>
       <c r="C201" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
@@ -13366,10 +13423,10 @@
         <v>248</v>
       </c>
       <c r="C202" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -13377,10 +13434,10 @@
         <v>248</v>
       </c>
       <c r="C203" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -13388,10 +13445,10 @@
         <v>248</v>
       </c>
       <c r="C204" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -13402,7 +13459,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
@@ -13413,7 +13470,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>211</v>
       </c>
@@ -13424,7 +13481,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>212</v>
       </c>
@@ -13435,7 +13492,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>213</v>
       </c>
@@ -13446,7 +13503,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>214</v>
       </c>
@@ -13457,7 +13514,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>215</v>
       </c>
@@ -13468,7 +13525,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>216</v>
       </c>
@@ -13479,7 +13536,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>217</v>
       </c>
@@ -13490,7 +13547,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>218</v>
       </c>
@@ -13501,7 +13558,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>219</v>
       </c>
@@ -13512,7 +13569,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>220</v>
       </c>
@@ -13523,7 +13580,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>221</v>
       </c>
@@ -13534,7 +13591,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>222</v>
       </c>
@@ -13542,7 +13599,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>223</v>
       </c>
@@ -13553,7 +13610,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>224</v>
       </c>
@@ -13564,7 +13621,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>225</v>
       </c>
@@ -13575,7 +13632,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>226</v>
       </c>
@@ -13586,7 +13643,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>227</v>
       </c>
@@ -13594,12 +13651,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>229</v>
       </c>
@@ -13610,7 +13667,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>230</v>
       </c>
@@ -13621,7 +13678,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>231</v>
       </c>
@@ -13632,7 +13689,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>232</v>
       </c>
@@ -13643,7 +13700,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>233</v>
       </c>
@@ -13654,7 +13711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>234</v>
       </c>
@@ -13665,7 +13722,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>235</v>
       </c>
@@ -13676,12 +13733,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>237</v>
       </c>
@@ -13689,7 +13746,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>238</v>
       </c>
@@ -13700,7 +13757,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>239</v>
       </c>
@@ -13711,22 +13768,22 @@
         <v>249</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>243</v>
       </c>
@@ -13737,7 +13794,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>244</v>
       </c>
@@ -13748,12 +13805,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>246</v>
       </c>
@@ -13764,7 +13821,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>247</v>
       </c>

</xml_diff>

<commit_message>
add new project assignment:
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\Summer Research\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD24E24A-7671-4135-B4F9-B19C648FE817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF90A9EE-DF5A-46E8-8EFD-1F779DC60E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="276">
   <si>
     <t>project name</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>NO TEST</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -11653,8 +11656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12802,148 +12805,268 @@
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="B99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="B100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="B101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="B102" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B103" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="B104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="B105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="B106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="B107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C107" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="B109" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="B110" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="B111" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
updated data for 99-118
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF90A9EE-DF5A-46E8-8EFD-1F779DC60E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52DB3DA-669D-4974-A021-201683EA0B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="283">
   <si>
     <t>project name</t>
   </si>
@@ -853,6 +853,27 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>no git repo, project status: retired</t>
+  </si>
+  <si>
+    <t>no gir repo</t>
+  </si>
+  <si>
+    <t>becomes tons of sub projects, save for later</t>
+  </si>
+  <si>
+    <t>has 4 sub projects</t>
+  </si>
+  <si>
+    <t>Cannot find any mock import from GetInfo.java though there are files with imports according to AllMetrics.csv, and the files actually exists, perhaps because of gradle build</t>
+  </si>
+  <si>
+    <t>build failed</t>
+  </si>
+  <si>
+    <t>This one is a gradle but succeed</t>
   </si>
 </sst>
 </file>
@@ -876,12 +897,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -897,12 +924,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11656,14 +11688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -12833,6 +12866,9 @@
       <c r="C101" t="s">
         <v>275</v>
       </c>
+      <c r="D101" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
@@ -12845,15 +12881,18 @@
         <v>275</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C103" t="s">
-        <v>275</v>
+      <c r="C103" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -12943,6 +12982,9 @@
       <c r="C111" t="s">
         <v>275</v>
       </c>
+      <c r="D111" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
@@ -12954,8 +12996,11 @@
       <c r="C112" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
@@ -12966,7 +13011,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
@@ -12976,8 +13021,11 @@
       <c r="C114" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
@@ -12987,8 +13035,11 @@
       <c r="C115" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -12999,7 +13050,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -13010,7 +13061,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
@@ -13020,53 +13071,56 @@
       <c r="C118" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
Update projects ownership and corresponding data.
Also added new data for previous projects.
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,27 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wchwe\ResearchCode\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wx199\mock-usage\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE98AAE4-C47D-4139-81F6-C1CDB350FBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40CEE20-10F6-4659-8AA3-A0E56BEA9FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="305">
   <si>
     <t>project name</t>
   </si>
@@ -855,13 +850,91 @@
     <t>In Progress</t>
   </si>
   <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>no git repo, project status: retired</t>
+  </si>
+  <si>
+    <t>no gir repo</t>
+  </si>
+  <si>
+    <t>becomes tons of sub projects, save for later</t>
+  </si>
+  <si>
+    <t>has 4 sub projects</t>
+  </si>
+  <si>
+    <t>Cannot find any mock import from GetInfo.java though there are files with imports according to AllMetrics.csv, and the files actually exists, perhaps because of gradle build</t>
+  </si>
+  <si>
+    <t>build failed</t>
+  </si>
+  <si>
+    <t>This one is a gradle but succeed</t>
+  </si>
+  <si>
     <t>Chenhao</t>
   </si>
   <si>
-    <t>Git Fetch Error</t>
-  </si>
-  <si>
-    <t>Codec Issue</t>
+    <t>commons-beanutils</t>
+  </si>
+  <si>
+    <t>commons-bsf</t>
+  </si>
+  <si>
+    <t>commons-chain</t>
+  </si>
+  <si>
+    <t>commons-cli</t>
+  </si>
+  <si>
+    <t>commons-codec</t>
+  </si>
+  <si>
+    <t>commons-collections</t>
+  </si>
+  <si>
+    <t>commons-compress</t>
+  </si>
+  <si>
+    <t>commons-configuration</t>
+  </si>
+  <si>
+    <t>commons-crypto</t>
+  </si>
+  <si>
+    <t>commons-csv</t>
+  </si>
+  <si>
+    <t>commons-daemon</t>
+  </si>
+  <si>
+    <t>commons-dbcp</t>
+  </si>
+  <si>
+    <t>commons-dbutils</t>
+  </si>
+  <si>
+    <t>commons-digester</t>
+  </si>
+  <si>
+    <t>commons-email</t>
+  </si>
+  <si>
+    <t>commons-exec</t>
+  </si>
+  <si>
+    <t>commons-fileupload</t>
+  </si>
+  <si>
+    <t>commons-functor</t>
+  </si>
+  <si>
+    <t>commons-geometry</t>
+  </si>
+  <si>
+    <t>httpcomponents-client</t>
   </si>
 </sst>
 </file>
@@ -885,12 +958,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -906,12 +985,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2602,7 +2686,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>141990</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2645,7 +2729,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>138050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2688,7 +2772,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>138280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2731,7 +2815,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>135610</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2774,7 +2858,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>124050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2860,7 +2944,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
+      <xdr:rowOff>103830</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2903,7 +2987,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>99890</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2946,7 +3030,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>100120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2989,7 +3073,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>97450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3032,7 +3116,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>85890</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3118,7 +3202,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>65670</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3161,7 +3245,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>62090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3204,7 +3288,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>61960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3247,7 +3331,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>59290</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3290,7 +3374,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>48090</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3376,7 +3460,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3419,7 +3503,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3462,7 +3546,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3505,7 +3589,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3548,7 +3632,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3591,7 +3675,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3634,7 +3718,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3677,7 +3761,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3720,7 +3804,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3763,7 +3847,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3806,7 +3890,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3849,7 +3933,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3892,7 +3976,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3935,7 +4019,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3978,7 +4062,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4021,7 +4105,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4064,7 +4148,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4107,7 +4191,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4150,7 +4234,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4193,7 +4277,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4236,7 +4320,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4279,7 +4363,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4322,7 +4406,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4365,7 +4449,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4408,7 +4492,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4451,7 +4535,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4494,7 +4578,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4537,7 +4621,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4580,7 +4664,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4623,7 +4707,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4666,7 +4750,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4709,7 +4793,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4752,7 +4836,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4795,7 +4879,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4838,7 +4922,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4881,7 +4965,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4924,7 +5008,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>93</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4967,7 +5051,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5010,7 +5094,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5053,7 +5137,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5096,7 +5180,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5139,7 +5223,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5182,7 +5266,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5225,7 +5309,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>100</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5268,7 +5352,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5311,7 +5395,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5354,7 +5438,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5397,7 +5481,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>104</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5440,7 +5524,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5483,7 +5567,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5526,7 +5610,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5569,7 +5653,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5612,7 +5696,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>109</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5655,7 +5739,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5698,7 +5782,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5741,7 +5825,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>112</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5784,7 +5868,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>113</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5827,7 +5911,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>114</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5870,7 +5954,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5913,7 +5997,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5956,7 +6040,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5999,7 +6083,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>118</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6042,7 +6126,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>119</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6085,7 +6169,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6128,7 +6212,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>121</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6171,7 +6255,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6214,7 +6298,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6257,7 +6341,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6300,7 +6384,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6343,7 +6427,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>126</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6386,7 +6470,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6429,7 +6513,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6472,7 +6556,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6515,7 +6599,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6558,7 +6642,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>131</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6601,7 +6685,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6644,7 +6728,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6687,7 +6771,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6730,7 +6814,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>135</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6773,7 +6857,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>136</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6816,7 +6900,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>137</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6859,7 +6943,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>138</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6902,7 +6986,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6945,7 +7029,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6988,7 +7072,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7031,7 +7115,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>142</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7074,7 +7158,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7117,7 +7201,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>144</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7160,7 +7244,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>145</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7203,7 +7287,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7246,7 +7330,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7289,7 +7373,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7332,7 +7416,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>149</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7375,7 +7459,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7418,7 +7502,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>151</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7461,7 +7545,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>152</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7504,7 +7588,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7547,7 +7631,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>154</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7590,7 +7674,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7633,7 +7717,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7676,7 +7760,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7719,7 +7803,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7762,7 +7846,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>159</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7805,7 +7889,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>160</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7848,7 +7932,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>161</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7891,7 +7975,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7934,7 +8018,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>163</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7977,7 +8061,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>164</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8020,7 +8104,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>165</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8063,7 +8147,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>166</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8106,7 +8190,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8149,7 +8233,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>168</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8192,7 +8276,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8235,7 +8319,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8278,7 +8362,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>171</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8321,7 +8405,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8364,7 +8448,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8407,7 +8491,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>174</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8450,7 +8534,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8493,7 +8577,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>176</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8536,7 +8620,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>177</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8579,7 +8663,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>178</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8622,7 +8706,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>179</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8665,7 +8749,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8708,7 +8792,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8751,7 +8835,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8794,7 +8878,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8837,7 +8921,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>184</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8880,7 +8964,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>185</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8923,7 +9007,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8966,7 +9050,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9009,7 +9093,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>188</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9052,7 +9136,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>189</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9095,7 +9179,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>190</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9138,7 +9222,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>191</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9181,7 +9265,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9224,7 +9308,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9267,7 +9351,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>194</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9310,7 +9394,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9353,7 +9437,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9396,7 +9480,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>197</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9439,7 +9523,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>198</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9482,7 +9566,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>199</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9525,7 +9609,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9568,7 +9652,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9611,7 +9695,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>202</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9654,7 +9738,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>203</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9697,7 +9781,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>204</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9740,7 +9824,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>205</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9783,7 +9867,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>206</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9826,7 +9910,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>207</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9869,7 +9953,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9912,7 +9996,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>209</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9955,7 +10039,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>210</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9998,7 +10082,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10041,7 +10125,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>212</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10084,7 +10168,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10127,7 +10211,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>214</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10170,7 +10254,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10213,7 +10297,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>216</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10256,7 +10340,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>217</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10299,7 +10383,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10342,7 +10426,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>219</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10385,7 +10469,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>220</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10428,7 +10512,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>221</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10471,7 +10555,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>222</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10514,7 +10598,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>223</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10557,7 +10641,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>224</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10600,7 +10684,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>225</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10643,7 +10727,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>226</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10686,7 +10770,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10729,7 +10813,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>228</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10772,7 +10856,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>229</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10815,7 +10899,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>230</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10858,7 +10942,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>231</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10901,7 +10985,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>232</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10944,7 +11028,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>233</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10987,7 +11071,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>234</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11030,7 +11114,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>235</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11073,7 +11157,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>236</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11116,7 +11200,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>237</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11159,7 +11243,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>238</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11202,7 +11286,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>239</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11245,7 +11329,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>240</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11288,7 +11372,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>241</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11331,7 +11415,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>242</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>27510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11665,17 +11749,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.84375" customWidth="1"/>
+    <col min="1" max="1" width="35.90625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11686,7 +11770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -11697,7 +11781,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11708,7 +11792,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11719,7 +11803,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11730,7 +11814,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -11741,7 +11825,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11752,7 +11836,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11763,7 +11847,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11771,7 +11855,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11782,7 +11866,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -11793,7 +11877,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -11804,7 +11888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -11815,7 +11899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -11826,7 +11910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -11837,7 +11921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -11848,7 +11932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -11859,7 +11943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -11870,7 +11954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -11881,7 +11965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -11892,7 +11976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -11903,7 +11987,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11914,7 +11998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -11925,7 +12009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -11936,7 +12020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -11947,7 +12031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -11958,7 +12042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -11969,7 +12053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -11980,7 +12064,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -11991,7 +12075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -12002,7 +12086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -12013,7 +12097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -12024,7 +12108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -12035,7 +12119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -12046,7 +12130,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -12057,7 +12141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -12068,7 +12152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -12079,7 +12163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -12089,8 +12173,11 @@
       <c r="C38" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D38" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -12100,8 +12187,11 @@
       <c r="C39" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -12111,8 +12201,11 @@
       <c r="C40" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -12122,8 +12215,11 @@
       <c r="C41" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D41" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -12133,8 +12229,11 @@
       <c r="C42" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -12144,8 +12243,11 @@
       <c r="C43" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D43" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -12155,8 +12257,11 @@
       <c r="C44" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D44" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -12166,8 +12271,11 @@
       <c r="C45" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D45" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -12177,8 +12285,11 @@
       <c r="C46" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D46" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -12188,8 +12299,11 @@
       <c r="C47" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D47" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -12199,8 +12313,11 @@
       <c r="C48" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D48" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -12210,8 +12327,11 @@
       <c r="C49" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D49" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -12221,8 +12341,11 @@
       <c r="C50" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D50" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -12232,8 +12355,11 @@
       <c r="C51" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D51" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -12243,8 +12369,11 @@
       <c r="C52" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D52" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -12254,8 +12383,11 @@
       <c r="C53" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D53" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -12265,8 +12397,11 @@
       <c r="C54" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D54" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -12276,8 +12411,11 @@
       <c r="C55" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D55" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -12287,8 +12425,11 @@
       <c r="C56" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D56" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -12298,8 +12439,11 @@
       <c r="C57" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D57" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -12310,7 +12454,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -12321,7 +12465,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -12332,7 +12476,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -12343,7 +12487,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -12354,7 +12498,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -12365,7 +12509,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -12376,7 +12520,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -12387,7 +12531,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -12398,7 +12542,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -12409,7 +12553,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -12420,7 +12564,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -12431,7 +12575,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -12442,7 +12586,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -12453,7 +12597,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -12464,7 +12608,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -12475,7 +12619,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -12486,7 +12630,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -12497,7 +12641,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -12508,7 +12652,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -12519,7 +12663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -12530,7 +12674,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -12544,7 +12688,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -12558,7 +12702,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -12572,7 +12716,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -12586,7 +12730,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -12600,7 +12744,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -12614,7 +12758,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -12628,7 +12772,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -12642,7 +12786,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -12656,7 +12800,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -12670,7 +12814,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -12684,7 +12828,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -12698,7 +12842,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -12712,7 +12856,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -12726,7 +12870,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -12740,7 +12884,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -12754,7 +12898,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -12768,7 +12912,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -12782,7 +12926,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -12796,7 +12940,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -12810,483 +12954,630 @@
         <v>268</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" t="s">
+        <v>276</v>
+      </c>
+      <c r="D101" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A103" s="1" t="s">
+      <c r="B102" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B104" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B105" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B107" t="s">
+        <v>14</v>
+      </c>
+      <c r="C107" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B109" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B110" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" t="s">
+        <v>276</v>
+      </c>
+      <c r="D111" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" t="s">
+        <v>276</v>
+      </c>
+      <c r="D112" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B114" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" t="s">
+        <v>276</v>
+      </c>
+      <c r="D114" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>276</v>
+      </c>
+      <c r="D115" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B116" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>276</v>
+      </c>
+      <c r="D118" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B119" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B120" t="s">
-        <v>276</v>
-      </c>
-      <c r="C120" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B120" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B121" t="s">
-        <v>276</v>
-      </c>
-      <c r="C121" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B122" t="s">
-        <v>276</v>
-      </c>
-      <c r="C122" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B122" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B123" t="s">
-        <v>276</v>
-      </c>
-      <c r="C123" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B124" t="s">
-        <v>276</v>
-      </c>
-      <c r="C124" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B125" t="s">
-        <v>276</v>
-      </c>
-      <c r="C125" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B125" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B126" t="s">
-        <v>276</v>
-      </c>
-      <c r="C126" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B127" t="s">
-        <v>276</v>
-      </c>
-      <c r="C127" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B127" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B128" t="s">
-        <v>276</v>
-      </c>
-      <c r="C128" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B129" t="s">
-        <v>276</v>
-      </c>
-      <c r="C129" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B129" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B130" t="s">
-        <v>276</v>
-      </c>
-      <c r="C130" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B130" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B131" t="s">
-        <v>276</v>
-      </c>
-      <c r="C131" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B131" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B132" t="s">
-        <v>276</v>
-      </c>
-      <c r="C132" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B133" t="s">
-        <v>276</v>
-      </c>
-      <c r="C133" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B133" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B134" t="s">
-        <v>276</v>
-      </c>
-      <c r="C134" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B134" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B135" t="s">
-        <v>276</v>
-      </c>
-      <c r="C135" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B135" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B136" t="s">
-        <v>276</v>
-      </c>
-      <c r="C136" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B137" t="s">
-        <v>276</v>
+      <c r="B137" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C137" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B138" t="s">
-        <v>276</v>
+      <c r="B138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C138" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B139" t="s">
-        <v>276</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="B139" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C139" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B140" t="s">
-        <v>276</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="B140" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C140" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
@@ -13297,7 +13588,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
@@ -13305,7 +13596,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
@@ -13316,7 +13607,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
@@ -13327,7 +13618,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
@@ -13338,7 +13629,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
@@ -13349,7 +13640,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
@@ -13360,7 +13651,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -13371,7 +13662,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
@@ -13382,7 +13673,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -13393,7 +13684,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
@@ -13401,7 +13692,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
@@ -13412,7 +13703,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
@@ -13423,7 +13714,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
@@ -13434,7 +13725,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
@@ -13445,7 +13736,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
@@ -13453,7 +13744,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
@@ -13464,7 +13755,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
@@ -13475,7 +13766,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
@@ -13486,7 +13777,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
@@ -13497,7 +13788,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
@@ -13505,7 +13796,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
@@ -13516,7 +13807,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
@@ -13524,7 +13815,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
@@ -13535,7 +13826,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
@@ -13546,7 +13837,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
@@ -13557,7 +13848,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
@@ -13565,7 +13856,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
@@ -13576,7 +13867,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
@@ -13587,7 +13878,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
@@ -13598,7 +13889,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
@@ -13609,7 +13900,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
@@ -13620,7 +13911,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
@@ -13631,7 +13922,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
@@ -13642,7 +13933,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -13653,7 +13944,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -13664,7 +13955,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -13675,7 +13966,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
@@ -13686,7 +13977,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>211</v>
       </c>
@@ -13697,7 +13988,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>212</v>
       </c>
@@ -13708,7 +13999,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>213</v>
       </c>
@@ -13719,7 +14010,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>214</v>
       </c>
@@ -13730,7 +14021,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>215</v>
       </c>
@@ -13741,7 +14032,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>216</v>
       </c>
@@ -13752,7 +14043,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>217</v>
       </c>
@@ -13763,7 +14054,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>218</v>
       </c>
@@ -13774,7 +14065,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>219</v>
       </c>
@@ -13785,7 +14076,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>220</v>
       </c>
@@ -13796,7 +14087,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>221</v>
       </c>
@@ -13807,7 +14098,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>222</v>
       </c>
@@ -13815,7 +14106,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>223</v>
       </c>
@@ -13826,7 +14117,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>224</v>
       </c>
@@ -13837,7 +14128,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>225</v>
       </c>
@@ -13848,7 +14139,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>226</v>
       </c>
@@ -13859,7 +14150,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>227</v>
       </c>
@@ -13867,7 +14158,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>228</v>
       </c>
@@ -13875,7 +14166,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>229</v>
       </c>
@@ -13886,7 +14177,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>230</v>
       </c>
@@ -13897,7 +14188,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>231</v>
       </c>
@@ -13908,7 +14199,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>232</v>
       </c>
@@ -13919,7 +14210,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>233</v>
       </c>
@@ -13930,7 +14221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>234</v>
       </c>
@@ -13941,7 +14232,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>235</v>
       </c>
@@ -13952,7 +14243,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>236</v>
       </c>
@@ -13960,7 +14251,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>237</v>
       </c>
@@ -13971,7 +14262,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>238</v>
       </c>
@@ -13982,7 +14273,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>239</v>
       </c>
@@ -13993,7 +14284,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>240</v>
       </c>
@@ -14001,7 +14292,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>241</v>
       </c>
@@ -14009,7 +14300,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>242</v>
       </c>
@@ -14017,7 +14308,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>243</v>
       </c>
@@ -14028,7 +14319,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>244</v>
       </c>
@@ -14039,12 +14330,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>246</v>
       </c>
@@ -14055,7 +14346,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>247</v>
       </c>

</xml_diff>

<commit_message>
claim the new projects
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wx199\mock-usage\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wchwe\ResearchCode\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40CEE20-10F6-4659-8AA3-A0E56BEA9FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB89577-A2E0-4958-B813-C414F0D9ADC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41130" yWindow="3165" windowWidth="17400" windowHeight="16635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="305">
   <si>
     <t>project name</t>
   </si>
@@ -2686,7 +2686,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>141990</xdr:rowOff>
+      <xdr:rowOff>144712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2729,7 +2729,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>138050</xdr:rowOff>
+      <xdr:rowOff>132608</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2772,7 +2772,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>138280</xdr:rowOff>
+      <xdr:rowOff>132838</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2858,7 +2858,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>124050</xdr:rowOff>
+      <xdr:rowOff>121328</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2944,7 +2944,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>103830</xdr:rowOff>
+      <xdr:rowOff>106552</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2987,7 +2987,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>99890</xdr:rowOff>
+      <xdr:rowOff>94448</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3030,7 +3030,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>100120</xdr:rowOff>
+      <xdr:rowOff>94678</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3116,7 +3116,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>85890</xdr:rowOff>
+      <xdr:rowOff>83168</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3202,7 +3202,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>65670</xdr:rowOff>
+      <xdr:rowOff>68392</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3245,7 +3245,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>62090</xdr:rowOff>
+      <xdr:rowOff>56648</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3288,7 +3288,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>61960</xdr:rowOff>
+      <xdr:rowOff>56518</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3374,7 +3374,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>48090</xdr:rowOff>
+      <xdr:rowOff>45368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3460,7 +3460,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3503,7 +3503,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3546,7 +3546,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3589,7 +3589,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3632,7 +3632,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3675,7 +3675,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3718,7 +3718,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3761,7 +3761,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3804,7 +3804,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3847,7 +3847,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3890,7 +3890,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3933,7 +3933,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3976,7 +3976,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4019,7 +4019,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4062,7 +4062,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4105,7 +4105,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4148,7 +4148,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4191,7 +4191,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4234,7 +4234,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4277,7 +4277,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4320,7 +4320,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4363,7 +4363,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4406,7 +4406,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4449,7 +4449,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4492,7 +4492,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4535,7 +4535,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4578,7 +4578,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4621,7 +4621,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4664,7 +4664,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4707,7 +4707,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4750,7 +4750,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4793,7 +4793,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4836,7 +4836,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4879,7 +4879,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4922,7 +4922,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4965,7 +4965,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5008,7 +5008,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>93</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5051,7 +5051,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5094,7 +5094,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5137,7 +5137,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5180,7 +5180,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5223,7 +5223,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5266,7 +5266,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5309,7 +5309,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>100</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5352,7 +5352,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5395,7 +5395,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5438,7 +5438,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5481,7 +5481,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>104</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5524,7 +5524,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5567,7 +5567,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5610,7 +5610,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5653,7 +5653,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5696,7 +5696,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>109</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5739,7 +5739,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5782,7 +5782,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5825,7 +5825,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>112</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5868,7 +5868,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>113</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5911,7 +5911,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>114</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5954,7 +5954,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5997,7 +5997,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6040,7 +6040,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6083,7 +6083,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>118</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6126,7 +6126,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>119</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6169,7 +6169,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6212,7 +6212,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>121</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6255,7 +6255,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6298,7 +6298,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6341,7 +6341,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6384,7 +6384,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6427,7 +6427,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>126</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6470,7 +6470,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6513,7 +6513,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6556,7 +6556,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6599,7 +6599,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6642,7 +6642,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>131</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6685,7 +6685,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6728,7 +6728,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6771,7 +6771,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6814,7 +6814,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>135</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6857,7 +6857,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>136</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6900,7 +6900,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>137</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6943,7 +6943,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>138</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6986,7 +6986,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7029,7 +7029,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7072,7 +7072,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7115,7 +7115,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>142</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7158,7 +7158,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7201,7 +7201,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>144</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7244,7 +7244,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>145</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7287,7 +7287,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7330,7 +7330,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7373,7 +7373,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7416,7 +7416,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>149</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7459,7 +7459,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7502,7 +7502,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>151</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7545,7 +7545,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>152</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7588,7 +7588,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>153</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7631,7 +7631,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>154</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7674,7 +7674,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7717,7 +7717,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7760,7 +7760,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7803,7 +7803,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7846,7 +7846,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>159</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7889,7 +7889,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>160</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7932,7 +7932,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>161</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7975,7 +7975,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8018,7 +8018,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>163</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8061,7 +8061,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>164</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8104,7 +8104,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>165</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8147,7 +8147,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>166</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8190,7 +8190,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8233,7 +8233,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>168</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8276,7 +8276,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8319,7 +8319,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8362,7 +8362,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>171</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8405,7 +8405,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8448,7 +8448,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8491,7 +8491,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>174</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8534,7 +8534,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8577,7 +8577,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>176</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8620,7 +8620,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>177</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8663,7 +8663,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>178</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8706,7 +8706,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>179</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8749,7 +8749,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8792,7 +8792,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8835,7 +8835,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8878,7 +8878,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8921,7 +8921,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>184</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8964,7 +8964,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>185</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9007,7 +9007,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9050,7 +9050,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9093,7 +9093,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>188</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9136,7 +9136,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>189</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9179,7 +9179,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>190</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9222,7 +9222,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>191</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9265,7 +9265,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9308,7 +9308,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9351,7 +9351,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>194</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9394,7 +9394,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9437,7 +9437,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9480,7 +9480,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>197</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9523,7 +9523,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>198</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9566,7 +9566,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>199</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9609,7 +9609,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9652,7 +9652,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9695,7 +9695,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>202</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9738,7 +9738,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>203</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9781,7 +9781,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>204</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9824,7 +9824,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>205</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9867,7 +9867,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>206</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9910,7 +9910,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>207</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9953,7 +9953,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9996,7 +9996,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>209</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10039,7 +10039,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>210</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10082,7 +10082,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>211</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10125,7 +10125,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>212</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10168,7 +10168,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10211,7 +10211,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>214</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10254,7 +10254,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10297,7 +10297,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>216</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10340,7 +10340,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>217</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10383,7 +10383,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10426,7 +10426,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>219</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10469,7 +10469,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>220</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10512,7 +10512,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>221</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10555,7 +10555,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>222</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10598,7 +10598,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>223</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10641,7 +10641,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>224</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10684,7 +10684,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>225</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10727,7 +10727,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>226</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10770,7 +10770,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10813,7 +10813,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>228</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10856,7 +10856,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>229</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10899,7 +10899,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>230</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10942,7 +10942,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>231</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10985,7 +10985,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>232</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11028,7 +11028,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>233</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11071,7 +11071,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>234</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11114,7 +11114,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>235</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11157,7 +11157,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>236</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11200,7 +11200,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>237</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11243,7 +11243,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>238</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11286,7 +11286,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>239</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11329,7 +11329,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>240</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11372,7 +11372,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>241</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11415,7 +11415,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>151920</xdr:colOff>
       <xdr:row>242</xdr:row>
-      <xdr:rowOff>27510</xdr:rowOff>
+      <xdr:rowOff>30232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11749,17 +11749,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.90625" customWidth="1"/>
+    <col min="1" max="1" width="35.921875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11770,7 +11770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -11781,7 +11781,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11814,7 +11814,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -11866,7 +11866,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -11877,7 +11877,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -11888,7 +11888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -11921,7 +11921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -11998,7 +11998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -12031,7 +12031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -12042,7 +12042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -12075,7 +12075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -12086,7 +12086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -12119,7 +12119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -12141,7 +12141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -12152,7 +12152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -12191,7 +12191,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -12233,7 +12233,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -12261,7 +12261,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -12289,7 +12289,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -12303,7 +12303,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -12317,7 +12317,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -12331,7 +12331,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -12345,7 +12345,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -12359,7 +12359,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -12387,7 +12387,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -12401,7 +12401,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -12415,7 +12415,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -12429,7 +12429,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -12443,7 +12443,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -12465,7 +12465,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -12476,7 +12476,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -12487,7 +12487,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -12498,7 +12498,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -12509,7 +12509,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -12586,7 +12586,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -12597,7 +12597,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -12608,7 +12608,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -12619,7 +12619,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -12641,7 +12641,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -12663,7 +12663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -12674,7 +12674,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -12702,7 +12702,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -12758,7 +12758,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -12772,7 +12772,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -12786,7 +12786,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -12800,7 +12800,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -12814,7 +12814,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -12870,7 +12870,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -12898,7 +12898,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -12912,7 +12912,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -12940,7 +12940,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
@@ -12990,7 +12990,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
@@ -13001,7 +13001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
@@ -13070,7 +13070,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -13081,7 +13081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
@@ -13120,7 +13120,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
@@ -13131,7 +13131,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
@@ -13195,7 +13195,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
@@ -13206,7 +13206,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
@@ -13217,7 +13217,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
@@ -13228,7 +13228,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
@@ -13239,7 +13239,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
@@ -13250,7 +13250,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
@@ -13261,7 +13261,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
@@ -13283,7 +13283,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
@@ -13294,7 +13294,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
@@ -13305,7 +13305,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
@@ -13327,7 +13327,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -13338,7 +13338,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -13360,7 +13360,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
@@ -13393,7 +13393,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
@@ -13404,7 +13404,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
@@ -13415,7 +13415,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
@@ -13426,7 +13426,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
@@ -13437,147 +13437,195 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B141" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C141" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B142" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B143" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B144" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B145" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B146" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B147" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B148" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
@@ -13588,7 +13636,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
@@ -13596,7 +13644,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
@@ -13607,7 +13655,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
@@ -13618,7 +13666,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
@@ -13629,7 +13677,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
@@ -13640,7 +13688,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
@@ -13651,7 +13699,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -13662,7 +13710,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
@@ -13673,7 +13721,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -13684,7 +13732,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
@@ -13692,7 +13740,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
@@ -13703,7 +13751,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
@@ -13714,7 +13762,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
@@ -13725,7 +13773,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
@@ -13736,7 +13784,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
@@ -13744,7 +13792,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
@@ -13755,7 +13803,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
@@ -13766,7 +13814,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
@@ -13777,7 +13825,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
@@ -13788,7 +13836,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
@@ -13796,7 +13844,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
@@ -13807,7 +13855,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
@@ -13815,7 +13863,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
@@ -13826,7 +13874,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
@@ -13837,7 +13885,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
@@ -13848,7 +13896,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
@@ -13856,7 +13904,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
@@ -13867,7 +13915,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
@@ -13878,7 +13926,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
@@ -13889,7 +13937,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
@@ -13900,7 +13948,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
@@ -13911,7 +13959,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
@@ -13922,7 +13970,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
@@ -13933,7 +13981,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -13944,7 +13992,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -13955,7 +14003,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -13966,7 +14014,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
@@ -13977,7 +14025,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
         <v>211</v>
       </c>
@@ -13988,7 +14036,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
         <v>212</v>
       </c>
@@ -13999,7 +14047,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
         <v>213</v>
       </c>
@@ -14010,7 +14058,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
         <v>214</v>
       </c>
@@ -14021,7 +14069,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
         <v>215</v>
       </c>
@@ -14032,7 +14080,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
         <v>216</v>
       </c>
@@ -14043,7 +14091,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
         <v>217</v>
       </c>
@@ -14054,7 +14102,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
         <v>218</v>
       </c>
@@ -14065,7 +14113,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
         <v>219</v>
       </c>
@@ -14076,7 +14124,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
         <v>220</v>
       </c>
@@ -14087,7 +14135,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
         <v>221</v>
       </c>
@@ -14098,7 +14146,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
         <v>222</v>
       </c>
@@ -14106,7 +14154,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
         <v>223</v>
       </c>
@@ -14117,7 +14165,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
         <v>224</v>
       </c>
@@ -14128,7 +14176,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
         <v>225</v>
       </c>
@@ -14139,7 +14187,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
         <v>226</v>
       </c>
@@ -14150,7 +14198,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
         <v>227</v>
       </c>
@@ -14158,7 +14206,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
         <v>228</v>
       </c>
@@ -14166,7 +14214,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
         <v>229</v>
       </c>
@@ -14177,7 +14225,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
         <v>230</v>
       </c>
@@ -14188,7 +14236,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
         <v>231</v>
       </c>
@@ -14199,7 +14247,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
         <v>232</v>
       </c>
@@ -14210,7 +14258,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
         <v>233</v>
       </c>
@@ -14221,7 +14269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
         <v>234</v>
       </c>
@@ -14232,7 +14280,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
         <v>235</v>
       </c>
@@ -14243,7 +14291,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
         <v>236</v>
       </c>
@@ -14251,7 +14299,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
         <v>237</v>
       </c>
@@ -14262,7 +14310,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A234" s="1" t="s">
         <v>238</v>
       </c>
@@ -14273,7 +14321,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A235" s="1" t="s">
         <v>239</v>
       </c>
@@ -14284,7 +14332,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
         <v>240</v>
       </c>
@@ -14292,7 +14340,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
         <v>241</v>
       </c>
@@ -14300,7 +14348,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
         <v>242</v>
       </c>
@@ -14308,7 +14356,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
         <v>243</v>
       </c>
@@ -14319,7 +14367,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
         <v>244</v>
       </c>
@@ -14330,12 +14378,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
         <v>246</v>
       </c>
@@ -14346,7 +14394,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
         <v>247</v>
       </c>

</xml_diff>

<commit_message>
cleared data for build-failed projects
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22C5F7B-CFE5-4FDE-AE5F-81690675CA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71A4F66-AFAE-4C23-B10E-13D56B4A46A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12785,8 +12785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N152" sqref="N152"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K163" sqref="K163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added some more details on the project assignment sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\Summer Research\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E945D513-9F1B-40A7-A157-C217B18794F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6A23D7-1764-4CFD-846B-1D8C1D92670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="317">
   <si>
     <t>project name</t>
   </si>
@@ -983,6 +983,9 @@
   </si>
   <si>
     <t>SUM:</t>
+  </si>
+  <si>
+    <t>no mock import</t>
   </si>
 </sst>
 </file>
@@ -12785,8 +12788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13489,6 +13492,9 @@
       <c r="C58" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D58" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
@@ -13511,6 +13517,9 @@
       <c r="C60" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D60" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
@@ -13522,6 +13531,9 @@
       <c r="C61" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D61" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -13533,6 +13545,9 @@
       <c r="C62" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D62" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
@@ -13544,6 +13559,9 @@
       <c r="C63" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D63" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -13577,6 +13595,9 @@
       <c r="C66" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D66" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
@@ -13588,6 +13609,9 @@
       <c r="C67" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D67" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -13599,6 +13623,9 @@
       <c r="C68" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D68" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
@@ -13610,6 +13637,9 @@
       <c r="C69" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D69" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
@@ -13621,6 +13651,9 @@
       <c r="C70" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D70" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -13632,6 +13665,9 @@
       <c r="C71" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D71" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -13643,6 +13679,9 @@
       <c r="C72" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D72" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
@@ -13654,6 +13693,9 @@
       <c r="C73" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D73" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
@@ -13665,6 +13707,9 @@
       <c r="C74" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D74" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
@@ -13676,6 +13721,9 @@
       <c r="C75" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D75" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
@@ -13687,6 +13735,9 @@
       <c r="C76" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D76" s="5" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
@@ -13698,6 +13749,7 @@
       <c r="C77" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -13708,6 +13760,9 @@
       </c>
       <c r="C78" s="2" t="s">
         <v>252</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update project status, mark directory-studio as import failure
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6A23D7-1764-4CFD-846B-1D8C1D92670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C0BC01-FA29-4963-955F-BC41018104D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12788,8 +12788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14011,7 +14011,7 @@
         <v>42</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="D96" t="s">
         <v>271</v>

</xml_diff>

<commit_message>
Mark Drill project as import failure
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C0BC01-FA29-4963-955F-BC41018104D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3162A2-2B37-4D3D-94CA-886E856F3686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14025,7 +14025,7 @@
         <v>42</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="D97" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
Add project surfix for projects 119-138
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3162A2-2B37-4D3D-94CA-886E856F3686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E78C5D3-8D4B-40C6-8CD7-F6C62E9DE9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="336">
   <si>
     <t>project name</t>
   </si>
@@ -986,6 +986,63 @@
   </si>
   <si>
     <t>no mock import</t>
+  </si>
+  <si>
+    <t>guacamole-server</t>
+  </si>
+  <si>
+    <t>hama</t>
+  </si>
+  <si>
+    <t>harmony</t>
+  </si>
+  <si>
+    <t>hbase</t>
+  </si>
+  <si>
+    <t>helix</t>
+  </si>
+  <si>
+    <t>hive</t>
+  </si>
+  <si>
+    <t>hivemind</t>
+  </si>
+  <si>
+    <t>hop</t>
+  </si>
+  <si>
+    <t>httpcomponents</t>
+  </si>
+  <si>
+    <t>hudi</t>
+  </si>
+  <si>
+    <t>ignite</t>
+  </si>
+  <si>
+    <t>iotdb</t>
+  </si>
+  <si>
+    <t>isis</t>
+  </si>
+  <si>
+    <t>ivy</t>
+  </si>
+  <si>
+    <t>ivyde</t>
+  </si>
+  <si>
+    <t>jackrabbit</t>
+  </si>
+  <si>
+    <t>jakarta cactus</t>
+  </si>
+  <si>
+    <t>james</t>
+  </si>
+  <si>
+    <t>jclouds</t>
   </si>
 </sst>
 </file>
@@ -12788,8 +12845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14296,6 +14353,9 @@
       <c r="C119" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D119" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
@@ -14307,6 +14367,9 @@
       <c r="C120" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D120" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
@@ -14318,6 +14381,9 @@
       <c r="C121" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D121" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
@@ -14329,6 +14395,9 @@
       <c r="C122" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D122" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
@@ -14340,6 +14409,9 @@
       <c r="C123" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D123" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
@@ -14351,6 +14423,9 @@
       <c r="C124" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D124" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
@@ -14362,6 +14437,9 @@
       <c r="C125" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D125" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
@@ -14373,6 +14451,9 @@
       <c r="C126" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D126" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
@@ -14384,6 +14465,9 @@
       <c r="C127" s="5" t="s">
         <v>252</v>
       </c>
+      <c r="D127" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
@@ -14395,8 +14479,11 @@
       <c r="C128" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
@@ -14406,8 +14493,11 @@
       <c r="C129" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
@@ -14417,8 +14507,11 @@
       <c r="C130" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -14428,8 +14521,11 @@
       <c r="C131" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
@@ -14439,8 +14535,11 @@
       <c r="C132" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -14450,8 +14549,11 @@
       <c r="C133" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
@@ -14461,8 +14563,11 @@
       <c r="C134" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
@@ -14472,8 +14577,11 @@
       <c r="C135" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
@@ -14483,8 +14591,11 @@
       <c r="C136" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
@@ -14494,8 +14605,11 @@
       <c r="C137" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
@@ -14505,8 +14619,11 @@
       <c r="C138" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
@@ -14517,7 +14634,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
@@ -14528,7 +14645,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
@@ -14539,7 +14656,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
@@ -14550,7 +14667,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
@@ -14561,7 +14678,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Update project status, mark apache Jakarta Cactus as no git repo
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E78C5D3-8D4B-40C6-8CD7-F6C62E9DE9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD22E72-493F-42DF-9C4A-FA9A0893940F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,13 +1036,13 @@
     <t>jackrabbit</t>
   </si>
   <si>
-    <t>jakarta cactus</t>
-  </si>
-  <si>
     <t>james</t>
   </si>
   <si>
     <t>jclouds</t>
+  </si>
+  <si>
+    <t>no git repo</t>
   </si>
 </sst>
 </file>
@@ -12845,8 +12845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14589,10 +14589,10 @@
         <v>42</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D136" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -14606,7 +14606,7 @@
         <v>274</v>
       </c>
       <c r="D137" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -14620,7 +14620,7 @@
         <v>252</v>
       </c>
       <c r="D138" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update project assignment sheet as Guacamole cannot import
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD22E72-493F-42DF-9C4A-FA9A0893940F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9D37F1-1E5C-41BD-9FC7-529934D92FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1012,9 +1012,6 @@
     <t>hop</t>
   </si>
   <si>
-    <t>httpcomponents</t>
-  </si>
-  <si>
     <t>hudi</t>
   </si>
   <si>
@@ -1043,6 +1040,9 @@
   </si>
   <si>
     <t>no git repo</t>
+  </si>
+  <si>
+    <t>httpcomponents-core</t>
   </si>
 </sst>
 </file>
@@ -12845,8 +12845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14351,7 +14351,7 @@
         <v>42</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D119" t="s">
         <v>317</v>
@@ -14466,7 +14466,7 @@
         <v>252</v>
       </c>
       <c r="D127" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -14480,7 +14480,7 @@
         <v>252</v>
       </c>
       <c r="D128" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -14494,7 +14494,7 @@
         <v>252</v>
       </c>
       <c r="D129" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -14508,7 +14508,7 @@
         <v>252</v>
       </c>
       <c r="D130" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -14522,7 +14522,7 @@
         <v>252</v>
       </c>
       <c r="D131" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -14536,7 +14536,7 @@
         <v>252</v>
       </c>
       <c r="D132" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -14550,7 +14550,7 @@
         <v>252</v>
       </c>
       <c r="D133" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -14564,7 +14564,7 @@
         <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -14578,7 +14578,7 @@
         <v>252</v>
       </c>
       <c r="D135" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -14592,7 +14592,7 @@
         <v>250</v>
       </c>
       <c r="D136" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -14606,7 +14606,7 @@
         <v>274</v>
       </c>
       <c r="D137" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -14620,7 +14620,7 @@
         <v>252</v>
       </c>
       <c r="D138" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
extra detail for project 12-37 on assign sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9D37F1-1E5C-41BD-9FC7-529934D92FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE50323-5207-4294-A7AB-7FF2A438689F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="338">
   <si>
     <t>project name</t>
   </si>
@@ -1043,6 +1043,12 @@
   </si>
   <si>
     <t>httpcomponents-core</t>
+  </si>
+  <si>
+    <t>need to use a older version (release 1.9.2)</t>
+  </si>
+  <si>
+    <t>gradle</t>
   </si>
 </sst>
 </file>
@@ -12845,8 +12851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12855,7 +12861,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12866,7 +12872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -12877,7 +12883,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -12888,7 +12894,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -12899,7 +12905,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -12910,7 +12916,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -12921,7 +12927,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -12932,7 +12938,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -12943,7 +12949,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -12951,7 +12957,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -12962,7 +12968,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -12973,7 +12979,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -12984,7 +12990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -12995,7 +13001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -13006,7 +13012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -13017,7 +13023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -13027,8 +13033,11 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -13039,7 +13048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -13050,7 +13059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -13060,8 +13069,11 @@
       <c r="C19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -13072,7 +13084,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -13083,7 +13095,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -13094,7 +13106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -13105,7 +13117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -13116,7 +13128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -13126,8 +13138,11 @@
       <c r="C25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -13138,7 +13153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -13149,7 +13164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -13160,7 +13175,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -13171,7 +13186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -13182,7 +13197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -13193,7 +13208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Add data for projects 38-57, 79-98, 119-138
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE50323-5207-4294-A7AB-7FF2A438689F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82854F5B-0D72-4CB0-B5A4-BCD15D836709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12851,8 +12851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14365,8 +14365,8 @@
       <c r="B119" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C119" s="5" t="s">
-        <v>251</v>
+      <c r="C119" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="D119" t="s">
         <v>317</v>
@@ -14393,8 +14393,8 @@
       <c r="B121" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>252</v>
+      <c r="C121" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="D121" t="s">
         <v>319</v>
@@ -14450,7 +14450,7 @@
         <v>42</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D125" t="s">
         <v>323</v>
@@ -14547,8 +14547,8 @@
       <c r="B132" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>252</v>
+      <c r="C132" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="D132" t="s">
         <v>328</v>

</xml_diff>

<commit_message>
updated the project assignment sheet with more details
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82854F5B-0D72-4CB0-B5A4-BCD15D836709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B632557-EA75-4DE7-87C7-1D82530F65E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,9 +871,6 @@
     <t>no git repo, project status: retired</t>
   </si>
   <si>
-    <t>has 4 sub projects</t>
-  </si>
-  <si>
     <t>Cannot find any mock import from GetInfo.java though there are files with imports according to AllMetrics.csv, and the files actually exists, perhaps because of gradle build</t>
   </si>
   <si>
@@ -1049,6 +1046,9 @@
   </si>
   <si>
     <t>gradle</t>
+  </si>
+  <si>
+    <t>has 4 sub projects and doesn't use mocking framework</t>
   </si>
 </sst>
 </file>
@@ -12722,10 +12722,10 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -12736,7 +12736,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F4" s="9">
         <v>11</v>
@@ -12750,7 +12750,7 @@
         <v>93</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" s="9">
         <v>7</v>
@@ -12764,7 +12764,7 @@
         <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F6">
         <f>SUM(B5,B6)</f>
@@ -12779,7 +12779,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F7">
         <v>28</v>
@@ -12793,7 +12793,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F8" s="9">
         <v>16</v>
@@ -12807,7 +12807,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -12821,7 +12821,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F10">
         <f>SUM(F4:F9)</f>
@@ -12830,13 +12830,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B12" s="8">
         <v>231</v>
@@ -12851,8 +12851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13034,7 +13034,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -13070,7 +13070,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -13139,7 +13139,7 @@
         <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -13285,7 +13285,7 @@
         <v>252</v>
       </c>
       <c r="D38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -13299,7 +13299,7 @@
         <v>252</v>
       </c>
       <c r="D39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -13313,7 +13313,7 @@
         <v>252</v>
       </c>
       <c r="D40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -13327,7 +13327,7 @@
         <v>252</v>
       </c>
       <c r="D41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -13341,7 +13341,7 @@
         <v>252</v>
       </c>
       <c r="D42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -13355,7 +13355,7 @@
         <v>252</v>
       </c>
       <c r="D43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -13369,7 +13369,7 @@
         <v>252</v>
       </c>
       <c r="D44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -13383,7 +13383,7 @@
         <v>252</v>
       </c>
       <c r="D45" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -13397,7 +13397,7 @@
         <v>252</v>
       </c>
       <c r="D46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -13411,7 +13411,7 @@
         <v>252</v>
       </c>
       <c r="D47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -13425,7 +13425,7 @@
         <v>252</v>
       </c>
       <c r="D48" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -13439,7 +13439,7 @@
         <v>252</v>
       </c>
       <c r="D49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -13453,7 +13453,7 @@
         <v>252</v>
       </c>
       <c r="D50" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -13467,7 +13467,7 @@
         <v>252</v>
       </c>
       <c r="D51" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -13481,7 +13481,7 @@
         <v>252</v>
       </c>
       <c r="D52" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -13495,7 +13495,7 @@
         <v>252</v>
       </c>
       <c r="D53" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -13509,7 +13509,7 @@
         <v>252</v>
       </c>
       <c r="D54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -13523,7 +13523,7 @@
         <v>252</v>
       </c>
       <c r="D55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -13537,7 +13537,7 @@
         <v>252</v>
       </c>
       <c r="D56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -13551,7 +13551,7 @@
         <v>252</v>
       </c>
       <c r="D57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -13565,7 +13565,7 @@
         <v>252</v>
       </c>
       <c r="D58" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -13590,7 +13590,7 @@
         <v>252</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -13604,7 +13604,7 @@
         <v>252</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -13618,7 +13618,7 @@
         <v>252</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -13632,7 +13632,7 @@
         <v>252</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -13668,7 +13668,7 @@
         <v>252</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -13682,7 +13682,7 @@
         <v>252</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -13696,7 +13696,7 @@
         <v>252</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -13710,7 +13710,7 @@
         <v>252</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -13724,7 +13724,7 @@
         <v>252</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -13738,7 +13738,7 @@
         <v>252</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -13752,7 +13752,7 @@
         <v>252</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -13766,7 +13766,7 @@
         <v>252</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -13780,7 +13780,7 @@
         <v>252</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -13794,7 +13794,7 @@
         <v>252</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -13808,7 +13808,7 @@
         <v>252</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -13834,7 +13834,7 @@
         <v>252</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -14125,7 +14125,7 @@
         <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -14136,7 +14136,7 @@
         <v>14</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -14147,7 +14147,7 @@
         <v>14</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D101" t="s">
         <v>277</v>
@@ -14161,7 +14161,7 @@
         <v>14</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -14172,10 +14172,10 @@
         <v>14</v>
       </c>
       <c r="C103" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D103" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -14186,7 +14186,7 @@
         <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -14197,7 +14197,7 @@
         <v>14</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -14208,7 +14208,7 @@
         <v>14</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -14219,7 +14219,7 @@
         <v>14</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -14230,7 +14230,7 @@
         <v>14</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -14241,7 +14241,7 @@
         <v>14</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -14252,7 +14252,7 @@
         <v>14</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -14263,10 +14263,10 @@
         <v>14</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D111" t="s">
-        <v>278</v>
+        <v>337</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -14277,10 +14277,10 @@
         <v>14</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -14291,7 +14291,7 @@
         <v>14</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -14302,10 +14302,10 @@
         <v>14</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D114" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -14316,10 +14316,10 @@
         <v>14</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D115" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -14330,7 +14330,7 @@
         <v>14</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -14341,7 +14341,7 @@
         <v>14</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -14352,10 +14352,10 @@
         <v>14</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D118" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -14369,7 +14369,7 @@
         <v>273</v>
       </c>
       <c r="D119" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -14383,7 +14383,7 @@
         <v>252</v>
       </c>
       <c r="D120" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -14397,7 +14397,7 @@
         <v>273</v>
       </c>
       <c r="D121" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -14411,7 +14411,7 @@
         <v>252</v>
       </c>
       <c r="D122" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -14425,7 +14425,7 @@
         <v>252</v>
       </c>
       <c r="D123" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -14439,7 +14439,7 @@
         <v>252</v>
       </c>
       <c r="D124" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -14453,7 +14453,7 @@
         <v>250</v>
       </c>
       <c r="D125" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -14467,7 +14467,7 @@
         <v>252</v>
       </c>
       <c r="D126" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -14481,7 +14481,7 @@
         <v>252</v>
       </c>
       <c r="D127" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -14495,7 +14495,7 @@
         <v>252</v>
       </c>
       <c r="D128" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -14509,7 +14509,7 @@
         <v>252</v>
       </c>
       <c r="D129" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -14523,7 +14523,7 @@
         <v>252</v>
       </c>
       <c r="D130" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -14537,7 +14537,7 @@
         <v>252</v>
       </c>
       <c r="D131" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -14551,7 +14551,7 @@
         <v>273</v>
       </c>
       <c r="D132" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -14565,7 +14565,7 @@
         <v>252</v>
       </c>
       <c r="D133" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -14579,7 +14579,7 @@
         <v>252</v>
       </c>
       <c r="D134" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -14593,7 +14593,7 @@
         <v>252</v>
       </c>
       <c r="D135" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -14607,7 +14607,7 @@
         <v>250</v>
       </c>
       <c r="D136" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -14621,7 +14621,7 @@
         <v>274</v>
       </c>
       <c r="D137" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -14635,7 +14635,7 @@
         <v>252</v>
       </c>
       <c r="D138" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -14643,7 +14643,7 @@
         <v>143</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>249</v>
@@ -14654,7 +14654,7 @@
         <v>144</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>249</v>
@@ -14665,7 +14665,7 @@
         <v>145</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>249</v>
@@ -14676,7 +14676,7 @@
         <v>146</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>249</v>
@@ -14687,7 +14687,7 @@
         <v>147</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>249</v>
@@ -14698,7 +14698,7 @@
         <v>148</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>249</v>
@@ -14709,7 +14709,7 @@
         <v>149</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>249</v>
@@ -14720,7 +14720,7 @@
         <v>150</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>249</v>
@@ -14731,7 +14731,7 @@
         <v>151</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>249</v>
@@ -14742,7 +14742,7 @@
         <v>152</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>249</v>
@@ -14756,7 +14756,7 @@
         <v>14</v>
       </c>
       <c r="C149" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -14767,7 +14767,7 @@
         <v>14</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -14778,7 +14778,7 @@
         <v>14</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -14789,7 +14789,7 @@
         <v>14</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -14800,7 +14800,7 @@
         <v>14</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -14811,7 +14811,7 @@
         <v>14</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -14822,7 +14822,7 @@
         <v>14</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -14833,7 +14833,7 @@
         <v>14</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -14844,7 +14844,7 @@
         <v>14</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -14855,7 +14855,7 @@
         <v>14</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added extra details on project assign sheet
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE67235-E4B2-4FC0-8FEB-733C6ED021ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A312AD13-EABB-42C4-AE8C-C6D96243B850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="338">
   <si>
     <t>project name</t>
   </si>
@@ -12851,8 +12851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14707,7 +14707,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
@@ -14718,7 +14718,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
@@ -14740,7 +14740,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
@@ -14751,7 +14751,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
@@ -14762,7 +14762,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
@@ -14773,7 +14773,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
@@ -14783,8 +14783,11 @@
       <c r="C151" s="5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
@@ -14795,7 +14798,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
@@ -14805,8 +14808,11 @@
       <c r="C153" s="5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
@@ -14817,7 +14823,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
@@ -14828,7 +14834,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
@@ -14839,7 +14845,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
@@ -14850,7 +14856,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
@@ -14860,8 +14866,11 @@
       <c r="C158" s="5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
@@ -14872,7 +14881,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
found RQ1 12-37 had issues and fixed it, also updated project assign sheet with more detail
</commit_message>
<xml_diff>
--- a/Apache java projects assignment.xlsx
+++ b/Apache java projects assignment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\Summer Research\MockResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\2021 summer general\MockResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD5AD79-8AA4-4CFA-8985-27DF3A3CB922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA3F90-307F-4575-8A5C-D9BDDED859B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Projects" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Projects!$A$1:$D$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Projects!$C$1:$C$243</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="339">
   <si>
     <t>project name</t>
   </si>
@@ -12857,8 +12857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12888,6 +12888,9 @@
       <c r="C2" t="s">
         <v>338</v>
       </c>
+      <c r="D2" t="s">
+        <v>315</v>
+      </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -12980,6 +12983,9 @@
       <c r="C10" s="5" t="s">
         <v>338</v>
       </c>
+      <c r="D10" t="s">
+        <v>315</v>
+      </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -12992,6 +12998,9 @@
       <c r="C11" s="5" t="s">
         <v>338</v>
       </c>
+      <c r="D11" t="s">
+        <v>315</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -15852,6 +15861,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C243" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>